<commit_message>
Add Assessment History Page and change Assessment page to RunningAssessment
</commit_message>
<xml_diff>
--- a/excel examples/bioDataExample.xlsx
+++ b/excel examples/bioDataExample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keyz\Desktop\readingspreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alikali Ojonugwa\Documents\React-Projectx\COMPUTER_BASED-ASSESSMENT\cbt\excel examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E9E164-EB79-4725-9579-6972B52C29F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,7 +353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
a jagged but working add assessment page :-)
</commit_message>
<xml_diff>
--- a/excel examples/bioDataExample.xlsx
+++ b/excel examples/bioDataExample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keyz\Desktop\readingspreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keyz\Documents\cbt\cbt-new\computer-based-assessment\excel examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,18 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>matric</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>exam</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>13ms1023</t>
+  </si>
+  <si>
+    <t>16me1033</t>
+  </si>
+  <si>
+    <t>Emmanuel Menyaga</t>
+  </si>
+  <si>
+    <t>mathematical sciences</t>
+  </si>
+  <si>
+    <t>Ojonugwa Justice Alikali</t>
   </si>
 </sst>
 </file>
@@ -353,34 +356,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>30</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new assesment functionality implementation
</commit_message>
<xml_diff>
--- a/excel examples/bioDataExample.xlsx
+++ b/excel examples/bioDataExample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>13ms1023</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t>Ojonugwa Justice Alikali</t>
+  </si>
+  <si>
+    <t>matric</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>ca</t>
   </si>
 </sst>
 </file>
@@ -356,45 +371,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1">
-        <v>400</v>
-      </c>
-      <c r="E1">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
         <v>300</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>30</v>
       </c>
     </row>

</xml_diff>